<commit_message>
Added main timesheet compose function
</commit_message>
<xml_diff>
--- a/services.xlsx
+++ b/services.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
   <si>
     <t>Дата</t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t>фис</t>
+  </si>
+  <si>
+    <t>Подготовка договора купли-продажи</t>
+  </si>
+  <si>
+    <t>ЭС</t>
+  </si>
+  <si>
+    <t>Поиск информации по отказу от капремонта</t>
   </si>
 </sst>
 </file>
@@ -376,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -457,6 +466,170 @@
       <c r="E4" t="s">
         <v>8</v>
       </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1">
+        <v>45023</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1">
+        <v>45023</v>
+      </c>
+      <c r="B6">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1">
+        <v>45026</v>
+      </c>
+      <c r="B7">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1">
+        <v>45026</v>
+      </c>
+      <c r="B8">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1">
+        <v>45026</v>
+      </c>
+      <c r="B9">
+        <v>17</v>
+      </c>
+      <c r="C9">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1">
+        <v>45029</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1">
+        <v>45030</v>
+      </c>
+      <c r="B11">
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="1"/>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="1"/>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="1"/>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="1"/>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added excel write module, MVP
</commit_message>
<xml_diff>
--- a/services.xlsx
+++ b/services.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="13">
   <si>
     <t>Дата</t>
   </si>
@@ -48,10 +48,13 @@
     <t>Подготовка договора купли-продажи</t>
   </si>
   <si>
-    <t>ЭС</t>
-  </si>
-  <si>
     <t>Поиск информации по отказу от капремонта</t>
+  </si>
+  <si>
+    <t>Тестовое задание</t>
+  </si>
+  <si>
+    <t>сенопласт</t>
   </si>
 </sst>
 </file>
@@ -385,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -565,9 +568,6 @@
       <c r="D10" t="s">
         <v>9</v>
       </c>
-      <c r="E10" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1">
@@ -580,56 +580,348 @@
         <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="1"/>
+      <c r="A12" s="1">
+        <v>45033</v>
+      </c>
+      <c r="B12">
+        <v>9.5</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="1"/>
+      <c r="A13" s="1">
+        <v>45033</v>
+      </c>
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="1"/>
+      <c r="A14" s="1">
+        <v>45033</v>
+      </c>
+      <c r="B14">
+        <v>14.5</v>
+      </c>
+      <c r="C14">
+        <v>15</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="1"/>
+      <c r="A15" s="1">
+        <v>45033</v>
+      </c>
+      <c r="B15">
+        <v>16</v>
+      </c>
+      <c r="C15">
+        <v>17</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="1"/>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="1"/>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="1"/>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="1"/>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="1"/>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" s="1"/>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" s="1"/>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" s="1"/>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" s="1"/>
+      <c r="A16" s="1">
+        <v>45034</v>
+      </c>
+      <c r="B16">
+        <v>9.5</v>
+      </c>
+      <c r="C16">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1">
+        <v>45034</v>
+      </c>
+      <c r="B17">
+        <v>11</v>
+      </c>
+      <c r="C17">
+        <v>12</v>
+      </c>
+      <c r="D17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1">
+        <v>45034</v>
+      </c>
+      <c r="B18">
+        <v>14.5</v>
+      </c>
+      <c r="C18">
+        <v>15</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1">
+        <v>45034</v>
+      </c>
+      <c r="B19">
+        <v>16</v>
+      </c>
+      <c r="C19">
+        <v>17</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1">
+        <v>45035</v>
+      </c>
+      <c r="B20">
+        <v>9.5</v>
+      </c>
+      <c r="C20">
+        <v>10</v>
+      </c>
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1">
+        <v>45035</v>
+      </c>
+      <c r="B21">
+        <v>11</v>
+      </c>
+      <c r="C21">
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1">
+        <v>45035</v>
+      </c>
+      <c r="B22">
+        <v>14.5</v>
+      </c>
+      <c r="C22">
+        <v>15</v>
+      </c>
+      <c r="D22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1">
+        <v>45035</v>
+      </c>
+      <c r="B23">
+        <v>16</v>
+      </c>
+      <c r="C23">
+        <v>17</v>
+      </c>
+      <c r="D23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1">
+        <v>45036</v>
+      </c>
+      <c r="B24">
+        <v>9.5</v>
+      </c>
+      <c r="C24">
+        <v>10</v>
+      </c>
+      <c r="D24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1">
+        <v>45036</v>
+      </c>
+      <c r="B25">
+        <v>11</v>
+      </c>
+      <c r="C25">
+        <v>12</v>
+      </c>
+      <c r="D25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1">
+        <v>45036</v>
+      </c>
+      <c r="B26">
+        <v>14.5</v>
+      </c>
+      <c r="C26">
+        <v>15</v>
+      </c>
+      <c r="D26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1">
+        <v>45036</v>
+      </c>
+      <c r="B27">
+        <v>16</v>
+      </c>
+      <c r="C27">
+        <v>17</v>
+      </c>
+      <c r="D27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1">
+        <v>45037</v>
+      </c>
+      <c r="B28">
+        <v>9.5</v>
+      </c>
+      <c r="C28">
+        <v>10</v>
+      </c>
+      <c r="D28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="1">
+        <v>45037</v>
+      </c>
+      <c r="B29">
+        <v>11</v>
+      </c>
+      <c r="C29">
+        <v>12</v>
+      </c>
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="1">
+        <v>45037</v>
+      </c>
+      <c r="B30">
+        <v>14.5</v>
+      </c>
+      <c r="C30">
+        <v>15</v>
+      </c>
+      <c r="D30" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="1">
+        <v>45037</v>
+      </c>
+      <c r="B31">
+        <v>16</v>
+      </c>
+      <c r="C31">
+        <v>17</v>
+      </c>
+      <c r="D31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>